<commit_message>
Fig and tab updates
</commit_message>
<xml_diff>
--- a/scoring/SE_Scoring/EDGI_exercise_scoresheet_SE.xlsx
+++ b/scoring/SE_Scoring/EDGI_exercise_scoresheet_SE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Library/CloudStorage/Dropbox/Papers/EDGI_Exercise_Validation/scoring/SE_Scoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B8E1CF-CEBA-634E-85AC-BA424750BE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9879B7-5A5C-3140-98AE-C9AF25F8A8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1680" yWindow="1340" windowWidth="29040" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1140" windowWidth="29040" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ED100k" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2903" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2913" uniqueCount="675">
   <si>
     <t>raw_vars</t>
   </si>
@@ -2045,6 +2045,21 @@
   </si>
   <si>
     <t>ED100k_binge == 0</t>
+  </si>
+  <si>
+    <t>gender, sex</t>
+  </si>
+  <si>
+    <t>ED100k_gender_dummy_2</t>
+  </si>
+  <si>
+    <t>Gender coded as Cisgender Female, Cisgender Male, or Gender Diverse</t>
+  </si>
+  <si>
+    <t>Cisgender Male = 0, Cisgender Female = 1, Gender Diverse = 2</t>
+  </si>
+  <si>
+    <t>gender == 1 &amp; sex == 1 ~ 0, gender == 2 &amp; sex == 2 ~ 1, sex == 1 &amp; gender &gt; 1 ~ 2, sex == 2 &amp; gender == 1 ~ 2, sex == 2 &amp; gender &gt; 2 ~2, sex == 3 ~ 2</t>
   </si>
 </sst>
 </file>
@@ -3175,10 +3190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B99" zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="119" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6349,83 +6364,83 @@
     </row>
     <row r="91" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="29" t="s">
-        <v>518</v>
+        <v>670</v>
       </c>
       <c r="B91" s="29" t="s">
-        <v>528</v>
+        <v>671</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>529</v>
+        <v>672</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>234</v>
+        <v>294</v>
       </c>
       <c r="E91" s="29">
         <v>4</v>
       </c>
       <c r="F91" s="29" t="s">
+        <v>673</v>
+      </c>
+      <c r="G91" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I91" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J91" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K91" s="29" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="29" t="s">
+        <v>518</v>
+      </c>
+      <c r="B92" s="29" t="s">
+        <v>528</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D92" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="E92" s="29">
+        <v>4</v>
+      </c>
+      <c r="F92" s="29" t="s">
         <v>517</v>
       </c>
-      <c r="G91" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H91" s="29" t="s">
+      <c r="G92" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" s="29" t="s">
         <v>535</v>
       </c>
-      <c r="I91" s="29">
-        <v>0</v>
-      </c>
-      <c r="J91" s="29" t="s">
+      <c r="I92" s="29">
+        <v>0</v>
+      </c>
+      <c r="J92" s="29" t="s">
         <v>541</v>
       </c>
-      <c r="K91" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D92" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E92" s="9">
-        <v>4</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>481</v>
-      </c>
-      <c r="G92" s="9" t="s">
-        <v>653</v>
-      </c>
-      <c r="H92" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I92" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J92" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K92" s="9" t="s">
+      <c r="K92" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>14</v>
@@ -6434,10 +6449,10 @@
         <v>4</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H93" s="9" t="s">
         <v>11</v>
@@ -6454,13 +6469,13 @@
     </row>
     <row r="94" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>14</v>
@@ -6469,10 +6484,10 @@
         <v>4</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H94" s="9" t="s">
         <v>11</v>
@@ -6489,13 +6504,13 @@
     </row>
     <row r="95" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>14</v>
@@ -6504,10 +6519,10 @@
         <v>4</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H95" s="9" t="s">
         <v>11</v>
@@ -6524,13 +6539,13 @@
     </row>
     <row r="96" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="9" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>14</v>
@@ -6539,10 +6554,10 @@
         <v>4</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H96" s="9" t="s">
         <v>11</v>
@@ -6557,15 +6572,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>14</v>
@@ -6574,10 +6589,10 @@
         <v>4</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H97" s="9" t="s">
         <v>11</v>
@@ -6592,15 +6607,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>14</v>
@@ -6608,11 +6623,11 @@
       <c r="E98" s="9">
         <v>4</v>
       </c>
-      <c r="F98" s="9" t="s">
-        <v>479</v>
+      <c r="F98" s="7" t="s">
+        <v>487</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="H98" s="9" t="s">
         <v>11</v>
@@ -6627,15 +6642,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>14</v>
@@ -6644,7 +6659,7 @@
         <v>4</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>507</v>
+        <v>479</v>
       </c>
       <c r="G99" s="9" t="s">
         <v>655</v>
@@ -6662,132 +6677,132 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E100" s="9">
+        <v>4</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="H100" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I100" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J100" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K100" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A101" s="9" t="s">
         <v>667</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B101" s="9" t="s">
         <v>666</v>
       </c>
-      <c r="C100" s="6" t="s">
+      <c r="C101" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D100" s="9" t="s">
+      <c r="D101" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="E100" s="9">
+      <c r="E101" s="9">
         <v>5</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F101" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="G100" t="s">
+      <c r="G101" t="s">
         <v>664</v>
       </c>
-      <c r="H100" s="9" t="s">
+      <c r="H101" s="9" t="s">
         <v>669</v>
       </c>
-      <c r="I100" s="9">
-        <v>0</v>
-      </c>
-      <c r="J100" s="9" t="s">
+      <c r="I101" s="9">
+        <v>0</v>
+      </c>
+      <c r="J101" s="9" t="s">
         <v>668</v>
       </c>
-      <c r="K100" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="29" t="s">
+      <c r="K101" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="B101" s="29" t="s">
+      <c r="B102" s="29" t="s">
         <v>545</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D101" s="29" t="s">
+      <c r="D102" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="29">
+      <c r="E102" s="29">
         <v>5</v>
       </c>
-      <c r="F101" s="29" t="s">
+      <c r="F102" s="29" t="s">
         <v>547</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G102" s="29" t="s">
         <v>548</v>
       </c>
-      <c r="H101" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="I101" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="J101" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K101" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
+      <c r="H102" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I102" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J102" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K102" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A103" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B103" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="D102" s="9" t="s">
+      <c r="D103" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="E102" s="9">
+      <c r="E103" s="9">
         <v>5</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="G102" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H102" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I102" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J102" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K102" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" ht="85" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>666</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>616</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E103" s="9">
-        <v>6</v>
       </c>
       <c r="F103" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="G103" t="s">
-        <v>664</v>
+      <c r="G103" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="H103" s="9" t="s">
         <v>11</v>
@@ -6799,18 +6814,18 @@
         <v>11</v>
       </c>
       <c r="K103" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>291</v>
+        <v>666</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>322</v>
+        <v>616</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D104" s="9" t="s">
         <v>14</v>
@@ -6818,11 +6833,11 @@
       <c r="E104" s="9">
         <v>6</v>
       </c>
-      <c r="F104" s="7" t="s">
-        <v>482</v>
-      </c>
-      <c r="G104" s="9" t="s">
-        <v>653</v>
+      <c r="F104" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="G104" t="s">
+        <v>664</v>
       </c>
       <c r="H104" s="9" t="s">
         <v>11</v>
@@ -6839,13 +6854,13 @@
     </row>
     <row r="105" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>14</v>
@@ -6853,11 +6868,11 @@
       <c r="E105" s="9">
         <v>6</v>
       </c>
-      <c r="F105" s="9" t="s">
-        <v>483</v>
+      <c r="F105" s="7" t="s">
+        <v>482</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="H105" s="9" t="s">
         <v>11</v>
@@ -6872,48 +6887,50 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>29</v>
+        <v>293</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>665</v>
+        <v>321</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>606</v>
+        <v>72</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>234</v>
+        <v>14</v>
       </c>
       <c r="E106" s="9">
         <v>6</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>615</v>
+        <v>483</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>11</v>
+        <v>656</v>
       </c>
       <c r="H106" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="I106" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I106" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J106" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="K106" s="9"/>
-    </row>
-    <row r="107" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K106" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
-        <v>302</v>
+        <v>29</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>303</v>
+        <v>665</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>606</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>234</v>
@@ -6922,7 +6939,7 @@
         <v>6</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>11</v>
+        <v>615</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>11</v>
@@ -6934,21 +6951,19 @@
         <v>0</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="K107" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+        <v>496</v>
+      </c>
+      <c r="K107" s="9"/>
+    </row>
+    <row r="108" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>71</v>
+        <v>304</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="D108" s="9" t="s">
         <v>234</v>
@@ -6969,7 +6984,7 @@
         <v>0</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K108" s="9" t="s">
         <v>11</v>
@@ -6977,13 +6992,13 @@
     </row>
     <row r="109" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>28</v>
+        <v>310</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>234</v>
@@ -7004,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>251</v>
+        <v>491</v>
       </c>
       <c r="K109" s="9" t="s">
         <v>11</v>
@@ -7012,13 +7027,13 @@
     </row>
     <row r="110" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D110" s="9" t="s">
         <v>234</v>
@@ -7039,7 +7054,7 @@
         <v>0</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="K110" s="9" t="s">
         <v>11</v>
@@ -7047,104 +7062,104 @@
     </row>
     <row r="111" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B111" s="9" t="s">
         <v>296</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>299</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="E111" s="9">
         <v>6</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>484</v>
+        <v>11</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>655</v>
+        <v>11</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I111" s="9" t="s">
-        <v>11</v>
+        <v>623</v>
+      </c>
+      <c r="I111" s="9">
+        <v>0</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>11</v>
+        <v>249</v>
       </c>
       <c r="K111" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
-        <v>26</v>
+        <v>296</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>234</v>
+        <v>14</v>
       </c>
       <c r="E112" s="9">
         <v>6</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>11</v>
+        <v>484</v>
       </c>
       <c r="G112" s="9" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="I112" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="I112" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>250</v>
+        <v>11</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>292</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>300</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>69</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="E113" s="9">
         <v>6</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>479</v>
+        <v>11</v>
       </c>
       <c r="G113" s="9" t="s">
-        <v>655</v>
+        <v>11</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I113" s="9" t="s">
-        <v>11</v>
+        <v>623</v>
+      </c>
+      <c r="I113" s="9">
+        <v>0</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>11</v>
+        <v>250</v>
       </c>
       <c r="K113" s="9" t="s">
         <v>11</v>
@@ -7152,74 +7167,74 @@
     </row>
     <row r="114" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="9" t="s">
-        <v>638</v>
+        <v>292</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>652</v>
+        <v>300</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>271</v>
+        <v>14</v>
       </c>
       <c r="E114" s="9">
         <v>6</v>
       </c>
-      <c r="F114" s="9"/>
-      <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
-      <c r="J114" s="9"/>
-      <c r="K114" s="9"/>
+      <c r="F114" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="G114" s="9" t="s">
+        <v>655</v>
+      </c>
+      <c r="H114" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I114" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J114" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K114" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="115" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>652</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E115" s="9">
+        <v>6</v>
+      </c>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="9"/>
+      <c r="K115" s="9"/>
+    </row>
+    <row r="116" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="9" t="s">
         <v>665</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B116" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="C115" s="6" t="s">
+      <c r="C116" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="D115" s="9" t="s">
+      <c r="D116" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="E115" s="9">
-        <v>7</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>479</v>
-      </c>
-      <c r="G115" s="9" t="s">
-        <v>655</v>
-      </c>
-      <c r="H115" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I115" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J115" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K115" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="B116" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="D116" s="9" t="s">
-        <v>294</v>
       </c>
       <c r="E116" s="9">
         <v>7</v>
@@ -7228,7 +7243,7 @@
         <v>479</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="H116" s="9" t="s">
         <v>11</v>
@@ -7240,16 +7255,18 @@
         <v>11</v>
       </c>
       <c r="K116" s="9" t="s">
-        <v>619</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="9"/>
+      <c r="A117" s="9" t="s">
+        <v>323</v>
+      </c>
       <c r="B117" s="9" t="s">
-        <v>599</v>
+        <v>319</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>495</v>
+        <v>312</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>294</v>
@@ -7258,7 +7275,7 @@
         <v>7</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>547</v>
+        <v>479</v>
       </c>
       <c r="G117" s="9" t="s">
         <v>11</v>
@@ -7273,18 +7290,16 @@
         <v>11</v>
       </c>
       <c r="K117" s="9" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="9" t="s">
-        <v>306</v>
-      </c>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="9"/>
       <c r="B118" s="9" t="s">
-        <v>318</v>
+        <v>599</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>307</v>
+        <v>495</v>
       </c>
       <c r="D118" s="9" t="s">
         <v>294</v>
@@ -7293,7 +7308,7 @@
         <v>7</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>479</v>
+        <v>547</v>
       </c>
       <c r="G118" s="9" t="s">
         <v>11</v>
@@ -7308,27 +7323,27 @@
         <v>11</v>
       </c>
       <c r="K118" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
         <v>306</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="E119" s="9">
         <v>7</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>11</v>
+        <v>479</v>
       </c>
       <c r="G119" s="9" t="s">
         <v>11</v>
@@ -7343,27 +7358,27 @@
         <v>11</v>
       </c>
       <c r="K119" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="9" t="s">
-        <v>628</v>
+        <v>306</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>620</v>
+        <v>317</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>607</v>
+        <v>309</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="E120" s="9">
         <v>7</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>547</v>
+        <v>11</v>
       </c>
       <c r="G120" s="9" t="s">
         <v>11</v>
@@ -7378,30 +7393,30 @@
         <v>11</v>
       </c>
       <c r="K120" s="9" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>304</v>
+        <v>628</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="C121" s="5" t="s">
-        <v>303</v>
+        <v>620</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>607</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>14</v>
+        <v>294</v>
       </c>
       <c r="E121" s="9">
         <v>7</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>479</v>
+        <v>547</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>655</v>
+        <v>11</v>
       </c>
       <c r="H121" s="9" t="s">
         <v>11</v>
@@ -7413,30 +7428,30 @@
         <v>11</v>
       </c>
       <c r="K121" s="9" t="s">
-        <v>11</v>
+        <v>625</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>493</v>
+        <v>305</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E122" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F122" s="9" t="s">
         <v>479</v>
       </c>
       <c r="G122" s="9" t="s">
-        <v>610</v>
+        <v>655</v>
       </c>
       <c r="H122" s="9" t="s">
         <v>11</v>
@@ -7451,14 +7466,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
         <v>236</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>622</v>
-      </c>
-      <c r="C123" s="6"/>
+        <v>621</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>493</v>
+      </c>
       <c r="D123" s="9" t="s">
         <v>14</v>
       </c>
@@ -7469,7 +7486,7 @@
         <v>479</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H123" s="9" t="s">
         <v>11</v>
@@ -7484,18 +7501,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>509</v>
+        <v>236</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>508</v>
-      </c>
+        <v>622</v>
+      </c>
+      <c r="C124" s="6"/>
       <c r="D124" s="9" t="s">
-        <v>294</v>
+        <v>14</v>
       </c>
       <c r="E124" s="9">
         <v>8</v>
@@ -7504,7 +7519,7 @@
         <v>479</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>11</v>
+        <v>611</v>
       </c>
       <c r="H124" s="9" t="s">
         <v>11</v>
@@ -7516,18 +7531,18 @@
         <v>11</v>
       </c>
       <c r="K124" s="9" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>324</v>
+        <v>509</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>311</v>
+        <v>508</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>294</v>
@@ -7536,7 +7551,7 @@
         <v>8</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>11</v>
+        <v>479</v>
       </c>
       <c r="G125" s="9" t="s">
         <v>11</v>
@@ -7551,27 +7566,27 @@
         <v>11</v>
       </c>
       <c r="K125" s="9" t="s">
-        <v>608</v>
+        <v>510</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>511</v>
+        <v>617</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>512</v>
+        <v>311</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>294</v>
       </c>
       <c r="E126" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>479</v>
+        <v>11</v>
       </c>
       <c r="G126" s="9" t="s">
         <v>11</v>
@@ -7586,27 +7601,27 @@
         <v>11</v>
       </c>
       <c r="K126" s="9" t="s">
-        <v>627</v>
+        <v>608</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>609</v>
+        <v>511</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>294</v>
       </c>
       <c r="E127" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>11</v>
+        <v>479</v>
       </c>
       <c r="G127" s="9" t="s">
         <v>11</v>
@@ -7621,18 +7636,18 @@
         <v>11</v>
       </c>
       <c r="K127" s="9" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>477</v>
+        <v>514</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>294</v>
@@ -7656,30 +7671,65 @@
         <v>11</v>
       </c>
       <c r="K128" s="9" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E129" s="9">
+        <v>10</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J129" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K129" s="9" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B136" s="9"/>
-    </row>
-    <row r="137" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="9"/>
     </row>
-    <row r="138" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="9"/>
     </row>
-    <row r="139" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="9"/>
     </row>
-    <row r="140" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="9"/>
     </row>
-    <row r="141" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="9"/>
     </row>
+    <row r="142" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B142" s="9"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K141">
-    <sortCondition ref="E97:E141"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K142">
+    <sortCondition ref="E98:E142"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9831,7 +9881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="19" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>102</v>
       </c>
@@ -10951,7 +11001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -11091,7 +11141,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>101</v>
       </c>

</xml_diff>